<commit_message>
Now the panels are divided into load cases and the stress is averaged
</commit_message>
<xml_diff>
--- a/data/yannis/panel_properties.xlsx
+++ b/data/yannis/panel_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da260913b9116b48/Desktop/Yannis/Studium/4.Semester/ASE2/ASE project/Exported_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ADEF72B-4F27-4969-BFAD-DE831464D40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{886BEFF1-EAAB-4CD7-BBC4-B9D4193B4B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{928A721C-6D8D-43C1-B994-ABE212B63024}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F4888CD-DA49-4189-9072-56E1E83889C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>elements</t>
-  </si>
-  <si>
-    <t>shortestside</t>
   </si>
   <si>
     <t>thickness</t>
   </si>
   <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>longestside</t>
+    <t>mass</t>
   </si>
 </sst>
 </file>
@@ -428,23 +422,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCB7993-9530-4B60-8EAA-558F82E1A2E8}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A7A84F-A8A8-4E1D-A532-FB1FF0F188B9}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E32"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,521 +446,335 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>200000</v>
-      </c>
-      <c r="E2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>200000</v>
-      </c>
-      <c r="E3">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>200000</v>
-      </c>
-      <c r="E4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>200000</v>
-      </c>
-      <c r="E5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>200000</v>
-      </c>
-      <c r="E6">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>200000</v>
-      </c>
-      <c r="E7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>200000</v>
-      </c>
-      <c r="E8">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>200000</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>200000</v>
-      </c>
-      <c r="E10">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>200000</v>
-      </c>
-      <c r="E11">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>200000</v>
-      </c>
-      <c r="E12">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>200000</v>
-      </c>
-      <c r="E13">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>200000</v>
-      </c>
-      <c r="E14">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>200000</v>
-      </c>
-      <c r="E15">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>200000</v>
-      </c>
-      <c r="E16">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>200000</v>
-      </c>
-      <c r="E17">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>200000</v>
-      </c>
-      <c r="E18">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>200000</v>
-      </c>
-      <c r="E19">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>200000</v>
-      </c>
-      <c r="E20">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>200000</v>
-      </c>
-      <c r="E21">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>200000</v>
-      </c>
-      <c r="E22">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>200000</v>
-      </c>
-      <c r="E23">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>200000</v>
-      </c>
-      <c r="E24">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>200000</v>
-      </c>
-      <c r="E25">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>200000</v>
-      </c>
-      <c r="E26">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>200000</v>
-      </c>
-      <c r="E27">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>200000</v>
-      </c>
-      <c r="E28">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>200000</v>
-      </c>
-      <c r="E29">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30">
-        <v>200000</v>
-      </c>
-      <c r="E30">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31">
-        <v>200000</v>
-      </c>
-      <c r="E31">
-        <v>250</v>
+        <v>5.4000000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>